<commit_message>
Day 2: Updated decrees.html with Folk’s Gains
</commit_message>
<xml_diff>
--- a/docs/sam_tutelage.xlsx
+++ b/docs/sam_tutelage.xlsx
@@ -463,200 +463,200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Programming and Data Structures</t>
+          <t>Physics</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Code tools like `raven_tally.py`—track resources, messages, automate rule.</t>
+          <t>Understand forces—catapult design, castle defenses—enhancing military precision.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Inefficient raven messaging; untracked supplies during winter sieges.</t>
+          <t>Siege warfare inefficiencies; weak fortifications against dragons or trebuchets.</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tracked ravens, stocked granaries</t>
+          <t>Stronger walls, fewer siege losses</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Calculate taxes, troop logistics—ensure fair rule, efficient supply lines.</t>
+          <t>Craft wildfire, fertilizers—control resources, boost agriculture, wield power.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Misallocated resources; inaccurate levies causing unrest among smallfolk.</t>
+          <t>Famine from poor harvests; lack of alchemical defenses against foes like Cersei’s wildfire plots.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Fair taxes, well-fed armies</t>
+          <t>More crops, wildfire to deter invaders</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Understand forces—catapult design, castle defenses—enhancing military precision.</t>
+          <t>Calculate taxes, troop logistics—ensure fair rule, efficient supply lines.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Siege warfare inefficiencies; weak fortifications against dragons or trebuchets.</t>
+          <t>Misallocated resources; inaccurate levies causing unrest among smallfolk.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Stronger walls, fewer siege losses</t>
+          <t>Fair taxes, well-fed armies</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Discrete Mathematics</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Craft wildfire, fertilizers—control resources, boost agriculture, wield power.</t>
+          <t>Model alliances, voting systems—optimize diplomacy, council decisions.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Famine from poor harvests; lack of alchemical defenses against foes like Cersei’s wildfire plots.</t>
+          <t>Feudal disputes; unclear succession lines fueling wars (e.g., War of the Five Kings).</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>More crops, wildfire to deter invaders</t>
+          <t>Peaceful alliances, clear succession</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Discrete Mathematics</t>
+          <t>Engineering Mathematics</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Model alliances, voting systems—optimize diplomacy, council decisions.</t>
+          <t>Design bridges, aqueducts—improve infrastructure, unify the realm.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Feudal disputes; unclear succession lines fueling wars (e.g., War of the Five Kings).</t>
+          <t>Broken trade routes; flooded Riverlands disrupting food supply.</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Peaceful alliances, clear succession</t>
+          <t>Better roads, steady food from aqueducts</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Engineering Mathematics</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Design bridges, aqueducts—improve infrastructure, unify the realm.</t>
+          <t>Build signaling systems (e.g., raven relays)—speed communication across kingdoms.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Broken trade routes; flooded Riverlands disrupting food supply.</t>
+          <t>Slow message delivery; miscommunication sparking rebellions (e.g., Robb’s campaigns).</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Better roads, steady food from aqueducts</t>
+          <t>Faster news, fewer rebellions</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Computer Organisation and Architecture</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Build signaling systems (e.g., raven relays)—speed communication across kingdoms.</t>
+          <t>Structure data flow—organize royal records, troop movements digitally.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Slow message delivery; miscommunication sparking rebellions (e.g., Robb’s campaigns).</t>
+          <t>Lost scrolls; chaotic command during battles like Blackwater.</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Faster news, fewer rebellions</t>
+          <t>Orderly records, swift battle commands</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Computer Organisation and Architecture</t>
+          <t>Programming and Data Structures</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Structure data flow—organize royal records, troop movements digitally.</t>
+          <t>Code tools like `raven_tally.py`—track resources, messages, automate rule.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lost scrolls; chaotic command during battles like Blackwater.</t>
+          <t>Inefficient raven messaging; untracked supplies during winter sieges.</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Orderly records, swift battle commands</t>
+          <t>Tracked ravens, stocked granaries</t>
         </is>
       </c>
     </row>
@@ -688,100 +688,100 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Database Management Systems</t>
+          <t>Theory of Computation</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Store folk's data—track taxes, fealties, harvests in a royal database.</t>
+          <t>Predict system limits—ensure scalable governance as kingdoms grow.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lost lineage records (e.g., Jon Snow’s claim); untracked grain stores leading to starvation.</t>
+          <t>Overstretched rule post-war; failing to manage expanded territories after Daenerys’s conquests.</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Known lineage, full granaries</t>
+          <t>Stable rule over vast lands</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Theory of Computation</t>
+          <t>Compiler Design</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Predict system limits—ensure scalable governance as kingdoms grow.</t>
+          <t>Translate decrees to code—standardize commands for maesters, lords.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Overstretched rule post-war; failing to manage expanded territories after Daenerys’s conquests.</t>
+          <t>Misinterpreted royal orders; inconsistent law enforcement across regions.</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Stable rule over vast lands</t>
+          <t>Clear laws, uniform justice</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Compiler Design</t>
+          <t>Operating Systems</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Translate decrees to code—standardize commands for maesters, lords.</t>
+          <t>Manage kingdom processes—allocate resources, prioritize tasks like a king’s OS.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Misinterpreted royal orders; inconsistent law enforcement across regions.</t>
+          <t>Overlapping duties among lords; resource hoarding by Houses like Lannister.</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Clear laws, uniform justice</t>
+          <t>Fair resource split, efficient tasks</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Operating Systems</t>
+          <t>Database Management Systems</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Manage kingdom processes—allocate resources, prioritize tasks like a king’s OS.</t>
+          <t>Store folk’s data—track taxes, fealties, harvests in a royal database.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Overlapping duties among lords; resource hoarding by Houses like Lannister.</t>
+          <t>Lost lineage records (e.g., Jon Snow’s claim); untracked grain stores leading to starvation.</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Fair resource split, efficient tasks</t>
+          <t>Known lineage, full granaries</t>
         </is>
       </c>
     </row>
@@ -838,50 +838,50 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mechanical Engineering</t>
+          <t>Robotics</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Build siege engines, water mills—strengthen war and peace efforts.</t>
+          <t>Automate labor—forge golems for fields, walls—ease burdens, bolster defenses.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Weak trebuchets failing at sieges; insufficient grain milling during winters.</t>
+          <t>Smallfolk exhaustion; crumbling defenses against invaders (e.g., Wildlings breaching the Wall).</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Stronger sieges, milled grain aplenty</t>
+          <t>Rested workers, unbreached walls</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Robotics</t>
+          <t>Mechanical Engineering</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Automate labor—forge golems for fields, walls—ease burdens, bolster defenses.</t>
+          <t>Build siege engines, water mills—strengthen war and peace efforts.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Smallfolk exhaustion; crumbling defenses against invaders (e.g., Wildlings breaching the Wall).</t>
+          <t>Weak trebuchets failing at sieges; insufficient grain milling during winters.</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Rested workers, unbreached walls</t>
+          <t>Stronger sieges, milled grain aplenty</t>
         </is>
       </c>
     </row>

</xml_diff>